<commit_message>
Last updated on 2025-04-24 11:39:29
</commit_message>
<xml_diff>
--- a/prototype/assets/e3systems-small.xlsx
+++ b/prototype/assets/e3systems-small.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arghya/prototype/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arghya/arghyadutta.github.io/prototype/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262CFFE4-26FE-9142-A3E0-CEFB5BED7709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71331D07-2C7D-C64C-A607-3E07D29D3BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="95">
   <si>
     <t>upt_acc</t>
   </si>
@@ -297,6 +297,15 @@
   </si>
   <si>
     <t>list of tuples for InterPro domains of the protein in the form (IPR ID, start, end)</t>
+  </si>
+  <si>
+    <t>A,B,C</t>
+  </si>
+  <si>
+    <t>D,E,F</t>
+  </si>
+  <si>
+    <t>substrates</t>
   </si>
 </sst>
 </file>
@@ -326,7 +335,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -349,13 +358,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -660,15 +683,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:H15"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,8 +716,11 @@
       <c r="H1" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -719,8 +745,11 @@
       <c r="H2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -745,8 +774,11 @@
       <c r="H3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -771,8 +803,11 @@
       <c r="H4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -797,8 +832,11 @@
       <c r="H5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -823,8 +861,11 @@
       <c r="H6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -849,8 +890,11 @@
       <c r="H7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -875,8 +919,11 @@
       <c r="H8" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -901,8 +948,11 @@
       <c r="H9" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -927,8 +977,11 @@
       <c r="H10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -953,8 +1006,11 @@
       <c r="H11" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -979,8 +1035,11 @@
       <c r="H12" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -1005,8 +1064,11 @@
       <c r="H13" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -1031,8 +1093,11 @@
       <c r="H14" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -1057,8 +1122,11 @@
       <c r="H15" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -1082,6 +1150,9 @@
       </c>
       <c r="H16" t="s">
         <v>52</v>
+      </c>
+      <c r="I16" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>